<commit_message>
Fact de rechazo de pedidos y layout de rechazo de pedidos + adiciones al manual
</commit_message>
<xml_diff>
--- a/excel/Analisis de Hojas de Ruta.xlsx
+++ b/excel/Analisis de Hojas de Ruta.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14520" windowHeight="6990" tabRatio="687" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="5715" windowHeight="6420" tabRatio="687" firstSheet="2" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Hojas de Ruta" sheetId="5" r:id="rId1"/>
@@ -16,12 +16,12 @@
   </sheets>
   <calcPr calcId="125725" calcMode="manual"/>
   <pivotCaches>
-    <pivotCache cacheId="133" r:id="rId7"/>
-    <pivotCache cacheId="139" r:id="rId8"/>
-    <pivotCache cacheId="142" r:id="rId9"/>
-    <pivotCache cacheId="145" r:id="rId10"/>
-    <pivotCache cacheId="160" r:id="rId11"/>
-    <pivotCache cacheId="163" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
+    <pivotCache cacheId="3" r:id="rId8"/>
+    <pivotCache cacheId="4" r:id="rId9"/>
+    <pivotCache cacheId="5" r:id="rId10"/>
+    <pivotCache cacheId="14" r:id="rId11"/>
+    <pivotCache cacheId="23" r:id="rId12"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="95">
   <si>
     <t>Rótulos de columna</t>
   </si>
@@ -283,6 +283,48 @@
   </si>
   <si>
     <t>Diciembre</t>
+  </si>
+  <si>
+    <t>11270</t>
+  </si>
+  <si>
+    <t>28462</t>
+  </si>
+  <si>
+    <t>Carlos Del Carpio</t>
+  </si>
+  <si>
+    <t>Carlos E. Vacadiez</t>
+  </si>
+  <si>
+    <t>Fabrica Venta</t>
+  </si>
+  <si>
+    <t>Herman Atala Menacho</t>
+  </si>
+  <si>
+    <t>Ivan Morales</t>
+  </si>
+  <si>
+    <t>Juan Carlos Vargas</t>
+  </si>
+  <si>
+    <t>Luis Alberto Soleto Dorado</t>
+  </si>
+  <si>
+    <t>Nelson Cobarruvias Avila</t>
+  </si>
+  <si>
+    <t>Rafael Cardona Almendras</t>
+  </si>
+  <si>
+    <t>Reddy Toledo</t>
+  </si>
+  <si>
+    <t>Rolando Eguez</t>
+  </si>
+  <si>
+    <t>Wilson Quintela Almaraz</t>
   </si>
 </sst>
 </file>
@@ -497,279 +539,6 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Sergio Moreno" refreshedDate="39826.49429386574" backgroundQuery="1" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="7">
-    <cacheField name="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" numFmtId="0" hierarchy="53" level="32767"/>
-    <cacheField name="[Tipo Cliente].[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" numFmtId="0" hierarchy="14" level="1">
-      <sharedItems count="3">
-        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Activo]" c="Activo"/>
-        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Excluyente]" c="Excluyente"/>
-        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Potencial]" c="Potencial"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano]" caption="Ano" numFmtId="0" hierarchy="4" level="1">
-      <sharedItems count="8">
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[0]" c=""/>
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2003]" c="2003"/>
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2004]" c="2004"/>
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2005]" c="2005"/>
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2006]" c="2006"/>
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2007]" c="2007"/>
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2008]" c="2008"/>
-        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2009]" c="2009"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Mes]" caption="Mes" numFmtId="0" hierarchy="4" level="2">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Fecha]" caption="Fecha" numFmtId="0" hierarchy="4" level="3">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Mes].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="4" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Fecha].[Mes]" caption="Mes" propertyName="Mes" numFmtId="0" hierarchy="4" level="3" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="54">
-    <cacheHierarchy uniqueName="[Cliente].[Cliente]" caption="Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Cliente].[All]" allUniqueName="[Cliente].[Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente]" caption="Caracteristica Cliente" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio]" caption="Mercado - Expendio" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha de Actualizacion.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha Registro.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="4" unbalanced="0">
-      <fieldsUsage count="4">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
-        <fieldUsage x="4"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona]" caption="Zona" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona].[All]" allUniqueName="[Cliente - Ubicacion].[Zona].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona - UV]" caption="Zona - UV" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" allUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito]" caption="Distrito" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector]" caption="Distrito - Ruta - Sector" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Ruta]" caption="Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Sector]" caption="Sector" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Supervisor Ruta]" caption="Supervisor Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha]" caption="Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intercalacion Cliente].[Intercalacion Cliente]" caption="Intercalacion Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" allUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" dimensionUniqueName="[Intercalacion Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" attribute="1" defaultMemberUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Cliente].[Cedula]" caption="Cedula" attribute="1" defaultMemberUniqueName="[Cliente].[Cedula].[All]" allUniqueName="[Cliente].[Cedula].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Cliente Ubicacionfk]" caption="Cliente Ubicacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" allUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Codigo Cliente]" caption="Codigo Cliente" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Cliente].[All]" allUniqueName="[Cliente].[Codigo Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Direccion]" caption="Direccion" attribute="1" defaultMemberUniqueName="[Cliente].[Direccion].[All]" allUniqueName="[Cliente].[Direccion].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Email]" caption="Email" attribute="1" defaultMemberUniqueName="[Cliente].[Email].[All]" allUniqueName="[Cliente].[Email].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Empresa Sucursal Agenciafk]" caption="Empresa Sucursal Agenciafk" attribute="1" defaultMemberUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" allUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Expendio Caracteristicafk]" caption="Expendio Caracteristicafk" attribute="1" defaultMemberUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" allUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Fecha Registrofk]" caption="Fecha Registrofk" attribute="1" defaultMemberUniqueName="[Cliente].[Fecha Registrofk].[All]" allUniqueName="[Cliente].[Fecha Registrofk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Fechade Actualizacionfk]" caption="Fechade Actualizacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" allUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[NIT]" caption="NIT" attribute="1" defaultMemberUniqueName="[Cliente].[NIT].[All]" allUniqueName="[Cliente].[NIT].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nombre Completo]" caption="Nombre Completo" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Completo].[All]" allUniqueName="[Cliente].[Nombre Completo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nombre Local]" caption="Nombre Local" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Local].[All]" allUniqueName="[Cliente].[Nombre Local].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Telefono]" caption="Telefono" attribute="1" defaultMemberUniqueName="[Cliente].[Telefono].[All]" allUniqueName="[Cliente].[Telefono].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica]" caption="Dim Cliente Expendio Caracteristica" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio]" caption="Tipo Expendio" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado]" caption="Tipo Mercado" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano]" caption="Cliente - Fecha de Actualizacion.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Dia]" caption="Cliente - Fecha de Actualizacion.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Fecha]" caption="Cliente - Fecha de Actualizacion.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[FechaId]" caption="Cliente - Fecha de Actualizacion.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Mes]" caption="Cliente - Fecha de Actualizacion.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano]" caption="Cliente - Fecha Registro.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Dia]" caption="Cliente - Fecha Registro.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Dia].[All]" allUniqueName="[Cliente - Fecha Registro].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Fecha]" caption="Cliente - Fecha Registro.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[FechaId]" caption="Cliente - Fecha Registro.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" allUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Mes]" caption="Cliente - Fecha Registro.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Mes].[All]" allUniqueName="[Cliente - Fecha Registro].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion]" caption="Dim Cliente Ubicacion" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" allUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Manzano]" caption="Manzano" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Manzano].[All]" allUniqueName="[Cliente - Ubicacion].[Manzano].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[UV]" caption="UV" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[UV].[All]" allUniqueName="[Cliente - Ubicacion].[UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector]" caption="Dim Distrito Ruta Sector" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK]" caption="EmpresaSucursalAgenciaFK" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" allUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano]" caption="Ano" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Dia]" caption="Dia" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" allUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Fecha]" caption="Fecha" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[FechaId]" caption="FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" allUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Mes]" caption="Mes" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" allUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Tipo Cliente].[Dim Tipo Cliente]" caption="Dim Tipo Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Cantidad de Hojas de Ruta]" caption="Cantidad de Hojas de Ruta" measure="1" displayFolder="" measureGroup="Hoja de Ruta" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" measure="1" displayFolder="" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="10">
-    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
-    <dimension name="Cliente - Expendio Caracteristica" uniqueName="[Cliente - Expendio Caracteristica]" caption="Cliente - Expendio Caracteristica"/>
-    <dimension name="Cliente - Fecha de Actualizacion" uniqueName="[Cliente - Fecha de Actualizacion]" caption="Cliente - Fecha de Actualizacion"/>
-    <dimension name="Cliente - Fecha Registro" uniqueName="[Cliente - Fecha Registro]" caption="Cliente - Fecha Registro"/>
-    <dimension name="Cliente - Ubicacion" uniqueName="[Cliente - Ubicacion]" caption="Cliente - Ubicacion"/>
-    <dimension name="Distrito Ruta Sector" uniqueName="[Distrito Ruta Sector]" caption="Distrito Ruta Sector"/>
-    <dimension name="Fecha Hoja de Ruta" uniqueName="[Fecha Hoja de Ruta]" caption="Fecha Hoja de Ruta"/>
-    <dimension name="Intercalacion Cliente" uniqueName="[Intercalacion Cliente]" caption="Intercalacion Cliente"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Tipo Cliente" uniqueName="[Tipo Cliente]" caption="Tipo Cliente"/>
-  </dimensions>
-  <measureGroups count="1">
-    <measureGroup name="Hoja de Ruta" caption="Hoja de Ruta"/>
-  </measureGroups>
-  <maps count="9">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-    <map measureGroup="0" dimension="3"/>
-    <map measureGroup="0" dimension="4"/>
-    <map measureGroup="0" dimension="5"/>
-    <map measureGroup="0" dimension="6"/>
-    <map measureGroup="0" dimension="7"/>
-    <map measureGroup="0" dimension="9"/>
-  </maps>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Sergio Moreno" refreshedDate="39826.494302662039" backgroundQuery="1" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
-  <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="5">
-    <cacheField name="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" numFmtId="0" hierarchy="53" level="32767"/>
-    <cacheField name="[Tipo Cliente].[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" numFmtId="0" hierarchy="14" level="1">
-      <sharedItems count="3">
-        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Activo]" c="Activo"/>
-        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Excluyente]" c="Excluyente"/>
-        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Potencial]" c="Potencial"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Cliente - Ubicacion].[Zona - UV].[Zona]" caption="Zona" numFmtId="0" hierarchy="6" level="1">
-      <sharedItems count="10">
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[0]" c="CENTRO"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[1]" c="NORTE"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[2]" c="NORESTE"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[3]" c="NOROESTE"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[4]" c="SUR"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[5]" c="SURESTE"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[6]" c="SUROESTE"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[7]" c="ESTE"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[8]" c="OESTE"/>
-        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[99]" c="OTRA ZONA"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Cliente - Ubicacion].[Zona - UV].[Unidad Vecinal (UV)]" caption="Unidad Vecinal (UV)" numFmtId="0" hierarchy="6" level="2">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-    <cacheField name="[Cliente - Ubicacion].[Zona - UV].[Unidad Vecinal (UV)].[Zona]" caption="Zona" propertyName="Zona" numFmtId="0" hierarchy="6" level="2" memberPropertyField="1">
-      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="54">
-    <cacheHierarchy uniqueName="[Cliente].[Cliente]" caption="Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Cliente].[All]" allUniqueName="[Cliente].[Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente]" caption="Caracteristica Cliente" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio]" caption="Mercado - Expendio" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha de Actualizacion.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha Registro.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona]" caption="Zona" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona].[All]" allUniqueName="[Cliente - Ubicacion].[Zona].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona - UV]" caption="Zona - UV" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" allUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="3" unbalanced="0">
-      <fieldsUsage count="3">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="2"/>
-        <fieldUsage x="3"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito]" caption="Distrito" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector]" caption="Distrito - Ruta - Sector" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Ruta]" caption="Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Sector]" caption="Sector" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Supervisor Ruta]" caption="Supervisor Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha]" caption="Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Intercalacion Cliente].[Intercalacion Cliente]" caption="Intercalacion Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" allUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" dimensionUniqueName="[Intercalacion Cliente]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" attribute="1" defaultMemberUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Cliente].[Cedula]" caption="Cedula" attribute="1" defaultMemberUniqueName="[Cliente].[Cedula].[All]" allUniqueName="[Cliente].[Cedula].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Cliente Ubicacionfk]" caption="Cliente Ubicacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" allUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Codigo Cliente]" caption="Codigo Cliente" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Cliente].[All]" allUniqueName="[Cliente].[Codigo Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Direccion]" caption="Direccion" attribute="1" defaultMemberUniqueName="[Cliente].[Direccion].[All]" allUniqueName="[Cliente].[Direccion].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Email]" caption="Email" attribute="1" defaultMemberUniqueName="[Cliente].[Email].[All]" allUniqueName="[Cliente].[Email].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Empresa Sucursal Agenciafk]" caption="Empresa Sucursal Agenciafk" attribute="1" defaultMemberUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" allUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Expendio Caracteristicafk]" caption="Expendio Caracteristicafk" attribute="1" defaultMemberUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" allUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Fecha Registrofk]" caption="Fecha Registrofk" attribute="1" defaultMemberUniqueName="[Cliente].[Fecha Registrofk].[All]" allUniqueName="[Cliente].[Fecha Registrofk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Fechade Actualizacionfk]" caption="Fechade Actualizacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" allUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[NIT]" caption="NIT" attribute="1" defaultMemberUniqueName="[Cliente].[NIT].[All]" allUniqueName="[Cliente].[NIT].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nombre Completo]" caption="Nombre Completo" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Completo].[All]" allUniqueName="[Cliente].[Nombre Completo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Nombre Local]" caption="Nombre Local" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Local].[All]" allUniqueName="[Cliente].[Nombre Local].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente].[Telefono]" caption="Telefono" attribute="1" defaultMemberUniqueName="[Cliente].[Telefono].[All]" allUniqueName="[Cliente].[Telefono].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica]" caption="Dim Cliente Expendio Caracteristica" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio]" caption="Tipo Expendio" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado]" caption="Tipo Mercado" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano]" caption="Cliente - Fecha de Actualizacion.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Dia]" caption="Cliente - Fecha de Actualizacion.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Fecha]" caption="Cliente - Fecha de Actualizacion.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[FechaId]" caption="Cliente - Fecha de Actualizacion.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Mes]" caption="Cliente - Fecha de Actualizacion.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano]" caption="Cliente - Fecha Registro.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Dia]" caption="Cliente - Fecha Registro.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Dia].[All]" allUniqueName="[Cliente - Fecha Registro].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Fecha]" caption="Cliente - Fecha Registro.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[FechaId]" caption="Cliente - Fecha Registro.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" allUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Mes]" caption="Cliente - Fecha Registro.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Mes].[All]" allUniqueName="[Cliente - Fecha Registro].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion]" caption="Dim Cliente Ubicacion" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" allUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Manzano]" caption="Manzano" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Manzano].[All]" allUniqueName="[Cliente - Ubicacion].[Manzano].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[UV]" caption="UV" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[UV].[All]" allUniqueName="[Cliente - Ubicacion].[UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector]" caption="Dim Distrito Ruta Sector" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK]" caption="EmpresaSucursalAgenciaFK" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" allUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano]" caption="Ano" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Dia]" caption="Dia" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" allUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Fecha]" caption="Fecha" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[FechaId]" caption="FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" allUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Mes]" caption="Mes" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" allUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Tipo Cliente].[Dim Tipo Cliente]" caption="Dim Tipo Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Cantidad de Hojas de Ruta]" caption="Cantidad de Hojas de Ruta" measure="1" displayFolder="" measureGroup="Hoja de Ruta" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" measure="1" displayFolder="" count="0" oneField="1">
-      <fieldsUsage count="1">
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="10">
-    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
-    <dimension name="Cliente - Expendio Caracteristica" uniqueName="[Cliente - Expendio Caracteristica]" caption="Cliente - Expendio Caracteristica"/>
-    <dimension name="Cliente - Fecha de Actualizacion" uniqueName="[Cliente - Fecha de Actualizacion]" caption="Cliente - Fecha de Actualizacion"/>
-    <dimension name="Cliente - Fecha Registro" uniqueName="[Cliente - Fecha Registro]" caption="Cliente - Fecha Registro"/>
-    <dimension name="Cliente - Ubicacion" uniqueName="[Cliente - Ubicacion]" caption="Cliente - Ubicacion"/>
-    <dimension name="Distrito Ruta Sector" uniqueName="[Distrito Ruta Sector]" caption="Distrito Ruta Sector"/>
-    <dimension name="Fecha Hoja de Ruta" uniqueName="[Fecha Hoja de Ruta]" caption="Fecha Hoja de Ruta"/>
-    <dimension name="Intercalacion Cliente" uniqueName="[Intercalacion Cliente]" caption="Intercalacion Cliente"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Tipo Cliente" uniqueName="[Tipo Cliente]" caption="Tipo Cliente"/>
-  </dimensions>
-  <measureGroups count="1">
-    <measureGroup name="Hoja de Ruta" caption="Hoja de Ruta"/>
-  </measureGroups>
-  <maps count="9">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="0" dimension="1"/>
-    <map measureGroup="0" dimension="2"/>
-    <map measureGroup="0" dimension="3"/>
-    <map measureGroup="0" dimension="4"/>
-    <map measureGroup="0" dimension="5"/>
-    <map measureGroup="0" dimension="6"/>
-    <map measureGroup="0" dimension="7"/>
-    <map measureGroup="0" dimension="9"/>
-  </maps>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Sergio Moreno" refreshedDate="39826.494313194446" backgroundQuery="1" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="7">
@@ -915,7 +684,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Sergio Moreno" refreshedDate="39826.494485532407" backgroundQuery="1" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="5">
@@ -1116,7 +885,7 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Sergio Moreno" refreshedDate="39826.494906481479" backgroundQuery="1" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="7">
@@ -1295,8 +1064,335 @@
 </pivotCacheDefinition>
 </file>
 
+<file path=xl/pivotCache/pivotCacheDefinition5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Sergio Moreno" refreshedDate="39830.459475462965" backgroundQuery="1" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="10">
+    <cacheField name="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" numFmtId="0" hierarchy="53" level="32767"/>
+    <cacheField name="[Tipo Cliente].[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" numFmtId="0" hierarchy="14" level="1">
+      <sharedItems count="3">
+        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Activo]" c="Activo"/>
+        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Excluyente]" c="Excluyente"/>
+        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Potencial]" c="Potencial"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Cliente - Ubicacion].[Zona - UV].[Zona]" caption="Zona" numFmtId="0" hierarchy="6" level="1">
+      <sharedItems count="10">
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[0]" c="CENTRO"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[1]" c="NORTE"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[2]" c="NORESTE"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[3]" c="NOROESTE"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[4]" c="SUR"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[5]" c="SURESTE"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[6]" c="SUROESTE"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[7]" c="ESTE"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[8]" c="OESTE"/>
+        <s v="[Cliente - Ubicacion].[Zona - UV].[Zona].&amp;[99]" c="OTRA ZONA"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Cliente - Ubicacion].[Zona - UV].[Unidad Vecinal (UV)]" caption="Unidad Vecinal (UV)" numFmtId="0" hierarchy="6" level="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Cliente - Ubicacion].[Zona - UV].[Unidad Vecinal (UV)].[Zona]" caption="Zona" propertyName="Zona" numFmtId="0" hierarchy="6" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito]" caption="Distrito" numFmtId="0" hierarchy="8" level="1">
+      <sharedItems count="8">
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[1.]" c="Preventa Estampada"/>
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[2.]" c="Preventa Popular"/>
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[3.]" c="Auto Vta. Estampada"/>
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[4.]" c="Auto Vta. Popular"/>
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[5.]" c="Auto Vta. Provincia"/>
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[6.]" c="Auto Vta.agen-colg."/>
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[7.]" c="Vta Esp/fca"/>
+        <s v="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Distrito].&amp;[9.]" c="Free Cola"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Ruta]" caption="Ruta" numFmtId="0" hierarchy="8" level="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Sector]" caption="Sector" numFmtId="0" hierarchy="8" level="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Ruta].[Distrito]" caption="Distrito" propertyName="Distrito" numFmtId="0" hierarchy="8" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[Sector].[Ruta]" caption="Ruta" propertyName="Ruta" numFmtId="0" hierarchy="8" level="3" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="54">
+    <cacheHierarchy uniqueName="[Cliente].[Cliente]" caption="Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Cliente].[All]" allUniqueName="[Cliente].[Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente]" caption="Caracteristica Cliente" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio]" caption="Mercado - Expendio" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha de Actualizacion.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha Registro.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona]" caption="Zona" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona].[All]" allUniqueName="[Cliente - Ubicacion].[Zona].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona - UV]" caption="Zona - UV" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" allUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="3" unbalanced="0">
+      <fieldsUsage count="3">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+        <fieldUsage x="3"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito]" caption="Distrito" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector]" caption="Distrito - Ruta - Sector" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="4" unbalanced="0">
+      <fieldsUsage count="4">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="5"/>
+        <fieldUsage x="6"/>
+        <fieldUsage x="7"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Ruta]" caption="Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Sector]" caption="Sector" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Supervisor Ruta]" caption="Supervisor Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha]" caption="Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intercalacion Cliente].[Intercalacion Cliente]" caption="Intercalacion Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" allUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" dimensionUniqueName="[Intercalacion Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" attribute="1" defaultMemberUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Cliente].[Cedula]" caption="Cedula" attribute="1" defaultMemberUniqueName="[Cliente].[Cedula].[All]" allUniqueName="[Cliente].[Cedula].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Cliente Ubicacionfk]" caption="Cliente Ubicacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" allUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Codigo Cliente]" caption="Codigo Cliente" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Cliente].[All]" allUniqueName="[Cliente].[Codigo Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Direccion]" caption="Direccion" attribute="1" defaultMemberUniqueName="[Cliente].[Direccion].[All]" allUniqueName="[Cliente].[Direccion].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Email]" caption="Email" attribute="1" defaultMemberUniqueName="[Cliente].[Email].[All]" allUniqueName="[Cliente].[Email].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Empresa Sucursal Agenciafk]" caption="Empresa Sucursal Agenciafk" attribute="1" defaultMemberUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" allUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Expendio Caracteristicafk]" caption="Expendio Caracteristicafk" attribute="1" defaultMemberUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" allUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Fecha Registrofk]" caption="Fecha Registrofk" attribute="1" defaultMemberUniqueName="[Cliente].[Fecha Registrofk].[All]" allUniqueName="[Cliente].[Fecha Registrofk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Fechade Actualizacionfk]" caption="Fechade Actualizacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" allUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[NIT]" caption="NIT" attribute="1" defaultMemberUniqueName="[Cliente].[NIT].[All]" allUniqueName="[Cliente].[NIT].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nombre Completo]" caption="Nombre Completo" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Completo].[All]" allUniqueName="[Cliente].[Nombre Completo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nombre Local]" caption="Nombre Local" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Local].[All]" allUniqueName="[Cliente].[Nombre Local].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Telefono]" caption="Telefono" attribute="1" defaultMemberUniqueName="[Cliente].[Telefono].[All]" allUniqueName="[Cliente].[Telefono].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica]" caption="Dim Cliente Expendio Caracteristica" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio]" caption="Tipo Expendio" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado]" caption="Tipo Mercado" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano]" caption="Cliente - Fecha de Actualizacion.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Dia]" caption="Cliente - Fecha de Actualizacion.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Fecha]" caption="Cliente - Fecha de Actualizacion.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[FechaId]" caption="Cliente - Fecha de Actualizacion.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Mes]" caption="Cliente - Fecha de Actualizacion.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano]" caption="Cliente - Fecha Registro.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Dia]" caption="Cliente - Fecha Registro.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Dia].[All]" allUniqueName="[Cliente - Fecha Registro].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Fecha]" caption="Cliente - Fecha Registro.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[FechaId]" caption="Cliente - Fecha Registro.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" allUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Mes]" caption="Cliente - Fecha Registro.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Mes].[All]" allUniqueName="[Cliente - Fecha Registro].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion]" caption="Dim Cliente Ubicacion" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" allUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Manzano]" caption="Manzano" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Manzano].[All]" allUniqueName="[Cliente - Ubicacion].[Manzano].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[UV]" caption="UV" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[UV].[All]" allUniqueName="[Cliente - Ubicacion].[UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector]" caption="Dim Distrito Ruta Sector" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK]" caption="EmpresaSucursalAgenciaFK" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" allUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano]" caption="Ano" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Dia]" caption="Dia" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" allUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Fecha]" caption="Fecha" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[FechaId]" caption="FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" allUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Mes]" caption="Mes" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" allUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Tipo Cliente].[Dim Tipo Cliente]" caption="Dim Tipo Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Cantidad de Hojas de Ruta]" caption="Cantidad de Hojas de Ruta" measure="1" displayFolder="" measureGroup="Hoja de Ruta" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" measure="1" displayFolder="" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="10">
+    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
+    <dimension name="Cliente - Expendio Caracteristica" uniqueName="[Cliente - Expendio Caracteristica]" caption="Cliente - Expendio Caracteristica"/>
+    <dimension name="Cliente - Fecha de Actualizacion" uniqueName="[Cliente - Fecha de Actualizacion]" caption="Cliente - Fecha de Actualizacion"/>
+    <dimension name="Cliente - Fecha Registro" uniqueName="[Cliente - Fecha Registro]" caption="Cliente - Fecha Registro"/>
+    <dimension name="Cliente - Ubicacion" uniqueName="[Cliente - Ubicacion]" caption="Cliente - Ubicacion"/>
+    <dimension name="Distrito Ruta Sector" uniqueName="[Distrito Ruta Sector]" caption="Distrito Ruta Sector"/>
+    <dimension name="Fecha Hoja de Ruta" uniqueName="[Fecha Hoja de Ruta]" caption="Fecha Hoja de Ruta"/>
+    <dimension name="Intercalacion Cliente" uniqueName="[Intercalacion Cliente]" caption="Intercalacion Cliente"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Tipo Cliente" uniqueName="[Tipo Cliente]" caption="Tipo Cliente"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Hoja de Ruta" caption="Hoja de Ruta"/>
+  </measureGroups>
+  <maps count="9">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+    <map measureGroup="0" dimension="3"/>
+    <map measureGroup="0" dimension="4"/>
+    <map measureGroup="0" dimension="5"/>
+    <map measureGroup="0" dimension="6"/>
+    <map measureGroup="0" dimension="7"/>
+    <map measureGroup="0" dimension="9"/>
+  </maps>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" saveData="0" refreshedBy="Sergio Moreno" refreshedDate="39830.460602430554" backgroundQuery="1" createdVersion="3" refreshedVersion="3" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="8">
+    <cacheField name="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" numFmtId="0" hierarchy="53" level="32767"/>
+    <cacheField name="[Tipo Cliente].[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" numFmtId="0" hierarchy="14" level="1">
+      <sharedItems count="3">
+        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Activo]" c="Activo"/>
+        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Excluyente]" c="Excluyente"/>
+        <s v="[Tipo Cliente].[Tipo Cliente].&amp;[Potencial]" c="Potencial"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano]" caption="Ano" numFmtId="0" hierarchy="4" level="1">
+      <sharedItems count="8">
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[0]" c=""/>
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2003]" c="2003"/>
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2004]" c="2004"/>
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2005]" c="2005"/>
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2006]" c="2006"/>
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2007]" c="2007"/>
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2008]" c="2008"/>
+        <s v="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Ano].&amp;[2009]" c="2009"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Mes]" caption="Mes" numFmtId="0" hierarchy="4" level="2">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Fecha]" caption="Fecha" numFmtId="0" hierarchy="4" level="3">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Mes].[Ano]" caption="Ano" propertyName="Ano" numFmtId="0" hierarchy="4" level="2" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[Fecha].[Mes]" caption="Mes" propertyName="Mes" numFmtId="0" hierarchy="4" level="3" memberPropertyField="1">
+      <sharedItems containsSemiMixedTypes="0" containsString="0"/>
+    </cacheField>
+    <cacheField name="[Distrito Ruta Sector].[Supervisor Ruta].[Supervisor Ruta]" caption="Supervisor Ruta" numFmtId="0" hierarchy="11" level="1">
+      <sharedItems count="14">
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[11270]" c="11270"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[28462]" c="28462"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Carlos Del Carpio]" c="Carlos Del Carpio"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Carlos E. Vacadiez]" c="Carlos E. Vacadiez"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Fabrica Venta]" c="Fabrica Venta"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Herman Atala Menacho]" c="Herman Atala Menacho"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Ivan Morales]" c="Ivan Morales"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Juan Carlos Vargas]" c="Juan Carlos Vargas"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Luis Alberto Soleto Dorado]" c="Luis Alberto Soleto Dorado"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Nelson Cobarruvias Avila]" c="Nelson Cobarruvias Avila"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Rafael Cardona Almendras]" c="Rafael Cardona Almendras"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Reddy Toledo]" c="Reddy Toledo"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Rolando Eguez]" c="Rolando Eguez"/>
+        <s v="[Distrito Ruta Sector].[Supervisor Ruta].&amp;[Wilson Quintela Almaraz]" c="Wilson Quintela Almaraz"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="54">
+    <cacheHierarchy uniqueName="[Cliente].[Cliente]" caption="Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente].[Cliente].[All]" allUniqueName="[Cliente].[Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente]" caption="Caracteristica Cliente" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Caracteristica Cliente].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio]" caption="Mercado - Expendio" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Mercado - Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha de Actualizacion.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha]" caption="Cliente - Fecha Registro.Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="4" unbalanced="0">
+      <fieldsUsage count="4">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="2"/>
+        <fieldUsage x="3"/>
+        <fieldUsage x="4"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona]" caption="Zona" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona].[All]" allUniqueName="[Cliente - Ubicacion].[Zona].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Zona - UV]" caption="Zona - UV" defaultMemberUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" allUniqueName="[Cliente - Ubicacion].[Zona - UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito]" caption="Distrito" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector]" caption="Distrito - Ruta - Sector" defaultMemberUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Distrito - Ruta - Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Ruta]" caption="Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Sector]" caption="Sector" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Supervisor Ruta]" caption="Supervisor Ruta" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" allUniqueName="[Distrito Ruta Sector].[Supervisor Ruta].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="7"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha]" caption="Ano -  Mes -  Fecha" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano -  Mes -  Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Intercalacion Cliente].[Intercalacion Cliente]" caption="Intercalacion Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" allUniqueName="[Intercalacion Cliente].[Intercalacion Cliente].[All]" dimensionUniqueName="[Intercalacion Cliente]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Tipo Cliente].[Tipo Cliente]" caption="Tipo Cliente" attribute="1" defaultMemberUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Cliente].[Cedula]" caption="Cedula" attribute="1" defaultMemberUniqueName="[Cliente].[Cedula].[All]" allUniqueName="[Cliente].[Cedula].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Cliente Ubicacionfk]" caption="Cliente Ubicacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" allUniqueName="[Cliente].[Cliente Ubicacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Codigo Cliente]" caption="Codigo Cliente" attribute="1" defaultMemberUniqueName="[Cliente].[Codigo Cliente].[All]" allUniqueName="[Cliente].[Codigo Cliente].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Direccion]" caption="Direccion" attribute="1" defaultMemberUniqueName="[Cliente].[Direccion].[All]" allUniqueName="[Cliente].[Direccion].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Email]" caption="Email" attribute="1" defaultMemberUniqueName="[Cliente].[Email].[All]" allUniqueName="[Cliente].[Email].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Empresa Sucursal Agenciafk]" caption="Empresa Sucursal Agenciafk" attribute="1" defaultMemberUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" allUniqueName="[Cliente].[Empresa Sucursal Agenciafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Expendio Caracteristicafk]" caption="Expendio Caracteristicafk" attribute="1" defaultMemberUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" allUniqueName="[Cliente].[Expendio Caracteristicafk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Fecha Registrofk]" caption="Fecha Registrofk" attribute="1" defaultMemberUniqueName="[Cliente].[Fecha Registrofk].[All]" allUniqueName="[Cliente].[Fecha Registrofk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Fechade Actualizacionfk]" caption="Fechade Actualizacionfk" attribute="1" defaultMemberUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" allUniqueName="[Cliente].[Fechade Actualizacionfk].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[NIT]" caption="NIT" attribute="1" defaultMemberUniqueName="[Cliente].[NIT].[All]" allUniqueName="[Cliente].[NIT].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nombre Completo]" caption="Nombre Completo" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Completo].[All]" allUniqueName="[Cliente].[Nombre Completo].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Nombre Local]" caption="Nombre Local" attribute="1" defaultMemberUniqueName="[Cliente].[Nombre Local].[All]" allUniqueName="[Cliente].[Nombre Local].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente].[Telefono]" caption="Telefono" attribute="1" defaultMemberUniqueName="[Cliente].[Telefono].[All]" allUniqueName="[Cliente].[Telefono].[All]" dimensionUniqueName="[Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica]" caption="Dim Cliente Expendio Caracteristica" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Dim Cliente Expendio Caracteristica].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio]" caption="Tipo Expendio" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Expendio].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado]" caption="Tipo Mercado" attribute="1" defaultMemberUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" allUniqueName="[Cliente - Expendio Caracteristica].[Tipo Mercado].[All]" dimensionUniqueName="[Cliente - Expendio Caracteristica]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Ano]" caption="Cliente - Fecha de Actualizacion.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Dia]" caption="Cliente - Fecha de Actualizacion.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Fecha]" caption="Cliente - Fecha de Actualizacion.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[FechaId]" caption="Cliente - Fecha de Actualizacion.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha de Actualizacion].[Mes]" caption="Cliente - Fecha de Actualizacion.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" allUniqueName="[Cliente - Fecha de Actualizacion].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha de Actualizacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Ano]" caption="Cliente - Fecha Registro.Ano" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Ano].[All]" allUniqueName="[Cliente - Fecha Registro].[Ano].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Dia]" caption="Cliente - Fecha Registro.Dia" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Dia].[All]" allUniqueName="[Cliente - Fecha Registro].[Dia].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Fecha]" caption="Cliente - Fecha Registro.Fecha" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" allUniqueName="[Cliente - Fecha Registro].[Fecha].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[FechaId]" caption="Cliente - Fecha Registro.FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" allUniqueName="[Cliente - Fecha Registro].[FechaId].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Fecha Registro].[Mes]" caption="Cliente - Fecha Registro.Mes" attribute="1" time="1" defaultMemberUniqueName="[Cliente - Fecha Registro].[Mes].[All]" allUniqueName="[Cliente - Fecha Registro].[Mes].[All]" dimensionUniqueName="[Cliente - Fecha Registro]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion]" caption="Dim Cliente Ubicacion" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" allUniqueName="[Cliente - Ubicacion].[Dim Cliente Ubicacion].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[Manzano]" caption="Manzano" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[Manzano].[All]" allUniqueName="[Cliente - Ubicacion].[Manzano].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cliente - Ubicacion].[UV]" caption="UV" attribute="1" defaultMemberUniqueName="[Cliente - Ubicacion].[UV].[All]" allUniqueName="[Cliente - Ubicacion].[UV].[All]" dimensionUniqueName="[Cliente - Ubicacion]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector]" caption="Dim Distrito Ruta Sector" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" allUniqueName="[Distrito Ruta Sector].[Dim Distrito Ruta Sector].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK]" caption="EmpresaSucursalAgenciaFK" attribute="1" defaultMemberUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" allUniqueName="[Distrito Ruta Sector].[EmpresaSucursalAgenciaFK].[All]" dimensionUniqueName="[Distrito Ruta Sector]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Ano]" caption="Ano" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" allUniqueName="[Fecha Hoja de Ruta].[Ano].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Dia]" caption="Dia" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" allUniqueName="[Fecha Hoja de Ruta].[Dia].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Fecha]" caption="Fecha" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" allUniqueName="[Fecha Hoja de Ruta].[Fecha].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[FechaId]" caption="FechaId" attribute="1" time="1" keyAttribute="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" allUniqueName="[Fecha Hoja de Ruta].[FechaId].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Fecha Hoja de Ruta].[Mes]" caption="Mes" attribute="1" time="1" defaultMemberUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" allUniqueName="[Fecha Hoja de Ruta].[Mes].[All]" dimensionUniqueName="[Fecha Hoja de Ruta]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Tipo Cliente].[Dim Tipo Cliente]" caption="Dim Tipo Cliente" attribute="1" keyAttribute="1" defaultMemberUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" allUniqueName="[Tipo Cliente].[Dim Tipo Cliente].[All]" dimensionUniqueName="[Tipo Cliente]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Cantidad de Hojas de Ruta]" caption="Cantidad de Hojas de Ruta" measure="1" displayFolder="" measureGroup="Hoja de Ruta" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Cantidad de Clientes]" caption="Cantidad de Clientes" measure="1" displayFolder="" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="10">
+    <dimension name="Cliente" uniqueName="[Cliente]" caption="Cliente"/>
+    <dimension name="Cliente - Expendio Caracteristica" uniqueName="[Cliente - Expendio Caracteristica]" caption="Cliente - Expendio Caracteristica"/>
+    <dimension name="Cliente - Fecha de Actualizacion" uniqueName="[Cliente - Fecha de Actualizacion]" caption="Cliente - Fecha de Actualizacion"/>
+    <dimension name="Cliente - Fecha Registro" uniqueName="[Cliente - Fecha Registro]" caption="Cliente - Fecha Registro"/>
+    <dimension name="Cliente - Ubicacion" uniqueName="[Cliente - Ubicacion]" caption="Cliente - Ubicacion"/>
+    <dimension name="Distrito Ruta Sector" uniqueName="[Distrito Ruta Sector]" caption="Distrito Ruta Sector"/>
+    <dimension name="Fecha Hoja de Ruta" uniqueName="[Fecha Hoja de Ruta]" caption="Fecha Hoja de Ruta"/>
+    <dimension name="Intercalacion Cliente" uniqueName="[Intercalacion Cliente]" caption="Intercalacion Cliente"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Tipo Cliente" uniqueName="[Tipo Cliente]" caption="Tipo Cliente"/>
+  </dimensions>
+  <measureGroups count="1">
+    <measureGroup name="Hoja de Ruta" caption="Hoja de Ruta"/>
+  </measureGroups>
+  <maps count="9">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="0" dimension="1"/>
+    <map measureGroup="0" dimension="2"/>
+    <map measureGroup="0" dimension="3"/>
+    <map measureGroup="0" dimension="4"/>
+    <map measureGroup="0" dimension="5"/>
+    <map measureGroup="0" dimension="6"/>
+    <map measureGroup="0" dimension="7"/>
+    <map measureGroup="0" dimension="9"/>
+  </maps>
+</pivotCacheDefinition>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="133" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A2:I13" firstHeaderRow="1" firstDataRow="3" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField dataField="1" showAll="0"/>
@@ -1477,7 +1573,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="145" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A2:E7" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -1621,9 +1717,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="142" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A2:E14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A2:E73" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="10">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="4">
@@ -1654,39 +1750,242 @@
       </items>
     </pivotField>
     <pivotField showAll="0" dataSourceSort="1" defaultSubtotal="0" showPropTip="1"/>
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1">
+      <items count="9">
+        <item c="1" x="0"/>
+        <item c="1" x="1"/>
+        <item c="1" x="2"/>
+        <item c="1" x="3"/>
+        <item c="1" x="4"/>
+        <item c="1" x="5"/>
+        <item c="1" x="6"/>
+        <item c="1" x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
+      <items count="1">
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0" dataSourceSort="1">
+      <items count="1">
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" dataSourceSort="1" defaultSubtotal="0" showPropTip="1"/>
+    <pivotField showAll="0" dataSourceSort="1" defaultSubtotal="0" showPropTip="1"/>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="5"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="70">
     <i>
       <x/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
     <i>
       <x v="1"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
     <i>
       <x v="2"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
     <i>
       <x v="3"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
     <i>
       <x v="4"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
     <i>
       <x v="5"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
     <i>
       <x v="6"/>
     </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="9"/>
+    </i>
     <i>
       <x v="7"/>
     </i>
-    <i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
       <x v="8"/>
     </i>
-    <i>
+    <i r="1">
       <x v="9"/>
     </i>
     <i t="grand">
@@ -1726,7 +2025,12 @@
       </mps>
     </pivotHierarchy>
     <pivotHierarchy/>
-    <pivotHierarchy/>
+    <pivotHierarchy>
+      <mps count="2">
+        <mp field="8"/>
+        <mp field="9"/>
+      </mps>
+    </pivotHierarchy>
     <pivotHierarchy/>
     <pivotHierarchy/>
     <pivotHierarchy/>
@@ -1774,7 +2078,8 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
+  <rowHierarchiesUsage count="2">
+    <rowHierarchyUsage hierarchyUsage="8"/>
     <rowHierarchyUsage hierarchyUsage="6"/>
   </rowHierarchiesUsage>
   <colHierarchiesUsage count="1">
@@ -1784,9 +2089,9 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="139" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
-  <location ref="A2:E12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
-  <pivotFields count="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="23" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+  <location ref="A2:E99" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="8">
     <pivotField dataField="1" showAll="0"/>
     <pivotField axis="axisCol" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
       <items count="4">
@@ -1821,33 +2126,314 @@
     </pivotField>
     <pivotField showAll="0" dataSourceSort="1" defaultSubtotal="0" showPropTip="1"/>
     <pivotField showAll="0" dataSourceSort="1" defaultSubtotal="0" showPropTip="1"/>
+    <pivotField axis="axisRow" allDrilled="1" showAll="0" dataSourceSort="1" defaultAttributeDrillState="1">
+      <items count="15">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
   </pivotFields>
-  <rowFields count="1">
+  <rowFields count="2">
+    <field x="7"/>
     <field x="2"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="96">
     <i>
       <x/>
     </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
     <i>
       <x v="1"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
     <i>
       <x v="2"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
     <i>
       <x v="3"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
     <i>
       <x v="4"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
     <i>
       <x v="5"/>
     </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
     <i>
       <x v="6"/>
     </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
     <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
       <x v="7"/>
     </i>
     <i t="grand">
@@ -1936,7 +2522,8 @@
     <pivotHierarchy dragToRow="0" dragToCol="0" dragToPage="0" dragToData="1"/>
   </pivotHierarchies>
   <pivotTableStyleInfo name="PivotStyleMedium7" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <rowHierarchiesUsage count="1">
+  <rowHierarchiesUsage count="2">
+    <rowHierarchyUsage hierarchyUsage="11"/>
     <rowHierarchyUsage hierarchyUsage="4"/>
   </rowHierarchiesUsage>
   <colHierarchiesUsage count="1">
@@ -1946,7 +2533,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="163" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A2:E24" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField dataField="1" showAll="0"/>
@@ -2157,7 +2744,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica4" cacheId="160" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica4" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="3" minRefreshableVersion="3" showCalcMbrs="0" useAutoFormatting="1" itemPrintTitles="1" createdVersion="3" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A2:E31" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="5">
     <pivotField dataField="1" showAll="0"/>
@@ -2676,7 +3263,7 @@
   <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2998,7 +3585,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3115,15 +3702,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E73"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
@@ -3162,188 +3749,1191 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1">
+        <v>14488</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
+        <v>3816</v>
+      </c>
+      <c r="E4" s="1">
+        <v>18303</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B5" s="1">
+        <v>393</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0</v>
+      </c>
+      <c r="D5" s="1">
+        <v>99</v>
+      </c>
+      <c r="E5" s="1">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="1">
+        <v>683</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>130</v>
+      </c>
+      <c r="E6" s="1">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="1">
+        <v>595</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>101</v>
+      </c>
+      <c r="E7" s="1">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>258</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>40</v>
+      </c>
+      <c r="E8" s="1">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1198</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>202</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1400</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1445</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>206</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1651</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="1">
+        <v>716</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="1">
+        <v>112</v>
+      </c>
+      <c r="E11" s="1">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1082</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>153</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1235</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="1">
+        <v>586</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+      <c r="D13" s="1">
+        <v>146</v>
+      </c>
+      <c r="E13" s="1">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="1">
+        <v>7532</v>
+      </c>
+      <c r="C14" s="1">
+        <v>0</v>
+      </c>
+      <c r="D14" s="1">
+        <v>2627</v>
+      </c>
+      <c r="E14" s="1">
+        <v>10158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B15" s="1">
+        <v>11030</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1577</v>
+      </c>
+      <c r="D15" s="1">
+        <v>5650</v>
+      </c>
+      <c r="E15" s="1">
+        <v>18257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="1">
+        <v>172</v>
+      </c>
+      <c r="C16" s="1">
+        <v>122</v>
+      </c>
+      <c r="D16" s="1">
+        <v>194</v>
+      </c>
+      <c r="E16" s="1">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="1">
+        <v>552</v>
+      </c>
+      <c r="C17" s="1">
+        <v>55</v>
+      </c>
+      <c r="D17" s="1">
+        <v>204</v>
+      </c>
+      <c r="E17" s="1">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1">
+        <v>462</v>
+      </c>
+      <c r="C18" s="1">
+        <v>44</v>
+      </c>
+      <c r="D18" s="1">
+        <v>190</v>
+      </c>
+      <c r="E18" s="1">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="1">
+        <v>206</v>
+      </c>
+      <c r="C19" s="1">
+        <v>21</v>
+      </c>
+      <c r="D19" s="1">
+        <v>72</v>
+      </c>
+      <c r="E19" s="1">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B20" s="1">
+        <v>1090</v>
+      </c>
+      <c r="C20" s="1">
+        <v>17</v>
+      </c>
+      <c r="D20" s="1">
+        <v>279</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1158</v>
+      </c>
+      <c r="C21" s="1">
+        <v>17</v>
+      </c>
+      <c r="D21" s="1">
+        <v>474</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1649</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="1">
+        <v>616</v>
+      </c>
+      <c r="C22" s="1">
+        <v>29</v>
+      </c>
+      <c r="D22" s="1">
+        <v>183</v>
+      </c>
+      <c r="E22" s="1">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B23" s="1">
+        <v>826</v>
+      </c>
+      <c r="C23" s="1">
+        <v>35</v>
+      </c>
+      <c r="D23" s="1">
+        <v>361</v>
+      </c>
+      <c r="E23" s="1">
+        <v>1222</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="1">
+        <v>443</v>
+      </c>
+      <c r="C24" s="1">
+        <v>60</v>
+      </c>
+      <c r="D24" s="1">
+        <v>229</v>
+      </c>
+      <c r="E24" s="1">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="1">
+        <v>5505</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1177</v>
+      </c>
+      <c r="D25" s="1">
+        <v>3464</v>
+      </c>
+      <c r="E25" s="1">
+        <v>10146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B26" s="1">
+        <v>2822</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>24</v>
+      </c>
+      <c r="E26" s="1">
+        <v>2845</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="1">
+        <v>88</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0</v>
+      </c>
+      <c r="E27" s="1">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B28" s="1">
+        <v>40</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="1">
         <v>424</v>
       </c>
-      <c r="C4" s="1">
-        <v>123</v>
-      </c>
-      <c r="D4" s="1">
-        <v>246</v>
-      </c>
-      <c r="E4" s="1">
-        <v>494</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="1">
+        <v>34</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="1">
+        <v>140</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>1</v>
+      </c>
+      <c r="E31" s="1">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="1">
+        <v>170</v>
+      </c>
+      <c r="C32" s="1">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="1">
+        <v>62</v>
+      </c>
+      <c r="C33" s="1">
+        <v>0</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="1">
+        <v>1864</v>
+      </c>
+      <c r="C34" s="1">
+        <v>0</v>
+      </c>
+      <c r="D34" s="1">
         <v>22</v>
       </c>
-      <c r="B5" s="1">
-        <v>843</v>
-      </c>
-      <c r="C5" s="1">
-        <v>55</v>
-      </c>
-      <c r="D5" s="1">
-        <v>293</v>
-      </c>
-      <c r="E5" s="1">
-        <v>904</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
-      <c r="A6" s="3" t="s">
+      <c r="E34" s="1">
+        <v>1886</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="1">
+        <v>2019</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0</v>
+      </c>
+      <c r="D35" s="1">
+        <v>40</v>
+      </c>
+      <c r="E35" s="1">
+        <v>2059</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B36" s="1">
+        <v>49</v>
+      </c>
+      <c r="C36" s="1">
+        <v>0</v>
+      </c>
+      <c r="D36" s="1">
+        <v>1</v>
+      </c>
+      <c r="E36" s="1">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B37" s="1">
+        <v>244</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0</v>
+      </c>
+      <c r="E37" s="1">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" s="1">
+        <v>1</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B39" s="1">
+        <v>97</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1</v>
+      </c>
+      <c r="E39" s="1">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" s="1">
+        <v>127</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0</v>
+      </c>
+      <c r="D40" s="1">
+        <v>17</v>
+      </c>
+      <c r="E40" s="1">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B41" s="1">
+        <v>61</v>
+      </c>
+      <c r="C41" s="1">
+        <v>0</v>
+      </c>
+      <c r="D41" s="1">
+        <v>1</v>
+      </c>
+      <c r="E41" s="1">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1440</v>
+      </c>
+      <c r="C42" s="1">
+        <v>0</v>
+      </c>
+      <c r="D42" s="1">
+        <v>20</v>
+      </c>
+      <c r="E42" s="1">
+        <v>1460</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B43" s="1">
+        <v>277</v>
+      </c>
+      <c r="C43" s="1">
+        <v>0</v>
+      </c>
+      <c r="D43" s="1">
+        <v>39</v>
+      </c>
+      <c r="E43" s="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B44" s="1">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1">
+        <v>0</v>
+      </c>
+      <c r="D44" s="1">
+        <v>0</v>
+      </c>
+      <c r="E44" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="1">
+        <v>1</v>
+      </c>
+      <c r="C45" s="1">
+        <v>0</v>
+      </c>
+      <c r="D45" s="1">
+        <v>0</v>
+      </c>
+      <c r="E45" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B46" s="1">
+        <v>275</v>
+      </c>
+      <c r="C46" s="1">
+        <v>0</v>
+      </c>
+      <c r="D46" s="1">
+        <v>39</v>
+      </c>
+      <c r="E46" s="1">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="1">
+        <v>173</v>
+      </c>
+      <c r="C47" s="1">
+        <v>0</v>
+      </c>
+      <c r="D47" s="1">
+        <v>13</v>
+      </c>
+      <c r="E47" s="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B48" s="1">
+        <v>2</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B49" s="1">
+        <v>2</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B50" s="1">
+        <v>2</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B51" s="1">
+        <v>1</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B52" s="1">
+        <v>3</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0</v>
+      </c>
+      <c r="E54" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56" s="1">
+        <v>1</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <v>1</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B57" s="1">
+        <v>157</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1">
+        <v>12</v>
+      </c>
+      <c r="E57" s="1">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B58" s="1">
+        <v>14</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0</v>
+      </c>
+      <c r="E58" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B59" s="1">
+        <v>1</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0</v>
+      </c>
+      <c r="E59" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B60" s="1">
+        <v>1</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0</v>
+      </c>
+      <c r="E60" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B61" s="1">
+        <v>12</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B62" s="1">
+        <v>18221</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>18221</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B63" s="1">
+        <v>486</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B64" s="1">
+        <v>811</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>811</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B65" s="1">
         <v>690</v>
       </c>
-      <c r="C6" s="1">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1">
-        <v>250</v>
-      </c>
-      <c r="E6" s="1">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="1">
-        <v>272</v>
-      </c>
-      <c r="C7" s="1">
-        <v>21</v>
-      </c>
-      <c r="D7" s="1">
-        <v>93</v>
-      </c>
-      <c r="E7" s="1">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
+      <c r="B66" s="1">
+        <v>297</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="1">
-        <v>1751</v>
-      </c>
-      <c r="C8" s="1">
-        <v>17</v>
-      </c>
-      <c r="D8" s="1">
-        <v>420</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1826</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
+      <c r="B67" s="1">
+        <v>1387</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>1387</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="1">
-        <v>1594</v>
-      </c>
-      <c r="C9" s="1">
-        <v>17</v>
-      </c>
-      <c r="D9" s="1">
-        <v>595</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1686</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
+      <c r="B68" s="1">
+        <v>1618</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="1">
-        <v>919</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B69" s="1">
+        <v>820</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>0</v>
+      </c>
+      <c r="E69" s="1">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B70" s="1">
+        <v>1224</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1">
+        <v>0</v>
+      </c>
+      <c r="E70" s="1">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1">
-        <v>248</v>
-      </c>
-      <c r="E10" s="1">
-        <v>971</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B11" s="1">
-        <v>1360</v>
-      </c>
-      <c r="C11" s="1">
-        <v>35</v>
-      </c>
-      <c r="D11" s="1">
-        <v>498</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1401</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B12" s="1">
-        <v>708</v>
-      </c>
-      <c r="C12" s="1">
-        <v>60</v>
-      </c>
-      <c r="D12" s="1">
-        <v>292</v>
-      </c>
-      <c r="E12" s="1">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5">
-      <c r="A13" s="3" t="s">
+      <c r="B71" s="1">
+        <v>730</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0</v>
+      </c>
+      <c r="D71" s="1">
+        <v>0</v>
+      </c>
+      <c r="E71" s="1">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="1">
-        <v>10693</v>
-      </c>
-      <c r="C13" s="1">
-        <v>1177</v>
-      </c>
-      <c r="D13" s="1">
-        <v>5019</v>
-      </c>
-      <c r="E13" s="1">
-        <v>12564</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" s="3" t="s">
+      <c r="B72" s="1">
+        <v>10158</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>10158</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="1">
-        <v>19254</v>
-      </c>
-      <c r="C14" s="1">
-        <v>1578</v>
-      </c>
-      <c r="D14" s="1">
-        <v>7954</v>
-      </c>
-      <c r="E14" s="1">
+      <c r="B73" s="1">
+        <v>21596</v>
+      </c>
+      <c r="C73" s="1">
+        <v>1577</v>
+      </c>
+      <c r="D73" s="1">
+        <v>7927</v>
+      </c>
+      <c r="E73" s="1">
         <v>21684</v>
       </c>
     </row>
@@ -3354,15 +4944,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
     <col min="2" max="2" width="20.7109375" customWidth="1"/>
     <col min="3" max="3" width="10.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.28515625" customWidth="1"/>
@@ -3401,150 +4991,1633 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>81</v>
       </c>
       <c r="B4" s="1">
         <v>1</v>
       </c>
       <c r="C4" s="1">
+        <v>0</v>
+      </c>
+      <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="1">
-        <v>9871</v>
-      </c>
       <c r="C5" s="1">
-        <v>790</v>
+        <v>0</v>
       </c>
       <c r="D5" s="1">
-        <v>3786</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>10975</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="1">
+        <v>173</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0</v>
+      </c>
+      <c r="D6" s="1">
+        <v>13</v>
+      </c>
+      <c r="E6" s="1">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="1">
+        <v>119</v>
+      </c>
+      <c r="C7" s="1">
+        <v>0</v>
+      </c>
+      <c r="D7" s="1">
+        <v>7</v>
+      </c>
+      <c r="E7" s="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B6" s="1">
-        <v>932</v>
-      </c>
-      <c r="C6" s="1">
-        <v>57</v>
-      </c>
-      <c r="D6" s="1">
-        <v>351</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
-      <c r="A7" s="3" t="s">
+      <c r="B8" s="1">
+        <v>8</v>
+      </c>
+      <c r="C8" s="1">
+        <v>0</v>
+      </c>
+      <c r="D8" s="1">
+        <v>4</v>
+      </c>
+      <c r="E8" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="1">
-        <v>1471</v>
-      </c>
-      <c r="C7" s="1">
-        <v>474</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1323</v>
-      </c>
-      <c r="E7" s="1">
-        <v>2235</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
-      <c r="A8" s="3" t="s">
+      <c r="B9" s="1">
+        <v>31</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>1</v>
+      </c>
+      <c r="E9" s="1">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="1">
-        <v>2692</v>
-      </c>
-      <c r="C8" s="1">
-        <v>108</v>
-      </c>
-      <c r="D8" s="1">
-        <v>928</v>
-      </c>
-      <c r="E8" s="1">
-        <v>2869</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
-      <c r="A9" s="3" t="s">
+      <c r="B10" s="1">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1">
+        <v>0</v>
+      </c>
+      <c r="D10" s="1">
+        <v>1</v>
+      </c>
+      <c r="E10" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="B9" s="1">
-        <v>1310</v>
-      </c>
-      <c r="C9" s="1">
-        <v>54</v>
-      </c>
-      <c r="D9" s="1">
-        <v>429</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1344</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
-      <c r="A10" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B10" s="1">
-        <v>2969</v>
-      </c>
-      <c r="C10" s="1">
-        <v>94</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1134</v>
-      </c>
-      <c r="E10" s="1">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
-      <c r="A11" s="3" t="s">
-        <v>17</v>
       </c>
       <c r="B11" s="1">
         <v>8</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
       <c r="D11" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E11" s="1">
         <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5</v>
+      </c>
+      <c r="C12" s="1">
+        <v>0</v>
+      </c>
+      <c r="D12" s="1">
+        <v>0</v>
+      </c>
+      <c r="E12" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2822</v>
+      </c>
+      <c r="C13" s="1">
+        <v>19</v>
+      </c>
+      <c r="D13" s="1">
+        <v>43</v>
+      </c>
+      <c r="E13" s="1">
+        <v>2864</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1705</v>
+      </c>
+      <c r="C14" s="1">
+        <v>13</v>
+      </c>
+      <c r="D14" s="1">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1">
+        <v>1739</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B15" s="1">
+        <v>8</v>
+      </c>
+      <c r="C15" s="1">
         <v>1</v>
       </c>
-      <c r="B12" s="1">
-        <v>19254</v>
-      </c>
-      <c r="C12" s="1">
-        <v>1578</v>
-      </c>
-      <c r="D12" s="1">
-        <v>7954</v>
-      </c>
-      <c r="E12" s="1">
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B16" s="1">
+        <v>156</v>
+      </c>
+      <c r="C16" s="1">
+        <v>0</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17" s="1">
+        <v>627</v>
+      </c>
+      <c r="C17" s="1">
+        <v>2</v>
+      </c>
+      <c r="D17" s="1">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B18" s="1">
+        <v>0</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1">
+        <v>0</v>
+      </c>
+      <c r="E18" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" s="1">
+        <v>326</v>
+      </c>
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="1">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="1">
+        <v>9246</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0</v>
+      </c>
+      <c r="D20" s="1">
+        <v>1155</v>
+      </c>
+      <c r="E20" s="1">
+        <v>9853</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="1">
+        <v>1</v>
+      </c>
+      <c r="C21" s="1">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4459</v>
+      </c>
+      <c r="C22" s="1">
+        <v>0</v>
+      </c>
+      <c r="D22" s="1">
+        <v>500</v>
+      </c>
+      <c r="E22" s="1">
+        <v>4740</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" s="1">
+        <v>410</v>
+      </c>
+      <c r="C23" s="1">
+        <v>0</v>
+      </c>
+      <c r="D23" s="1">
+        <v>38</v>
+      </c>
+      <c r="E23" s="1">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B24" s="1">
+        <v>839</v>
+      </c>
+      <c r="C24" s="1">
+        <v>0</v>
+      </c>
+      <c r="D24" s="1">
+        <v>279</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1019</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1237</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0</v>
+      </c>
+      <c r="D25" s="1">
+        <v>133</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1275</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="1">
+        <v>838</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0</v>
+      </c>
+      <c r="D26" s="1">
+        <v>54</v>
+      </c>
+      <c r="E26" s="1">
+        <v>865</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1455</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0</v>
+      </c>
+      <c r="D27" s="1">
+        <v>151</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1514</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="1">
+        <v>7</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0</v>
+      </c>
+      <c r="E28" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" s="1">
+        <v>14</v>
+      </c>
+      <c r="C29" s="1">
+        <v>0</v>
+      </c>
+      <c r="D29" s="1">
+        <v>0</v>
+      </c>
+      <c r="E29" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B30" s="1">
+        <v>13</v>
+      </c>
+      <c r="C30" s="1">
+        <v>0</v>
+      </c>
+      <c r="D30" s="1">
+        <v>0</v>
+      </c>
+      <c r="E30" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1</v>
+      </c>
+      <c r="C31" s="1">
+        <v>0</v>
+      </c>
+      <c r="D31" s="1">
+        <v>0</v>
+      </c>
+      <c r="E31" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="1">
+        <v>3845</v>
+      </c>
+      <c r="C32" s="1">
+        <v>705</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1678</v>
+      </c>
+      <c r="E32" s="1">
+        <v>6228</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1909</v>
+      </c>
+      <c r="C33" s="1">
+        <v>391</v>
+      </c>
+      <c r="D33" s="1">
+        <v>865</v>
+      </c>
+      <c r="E33" s="1">
+        <v>3165</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="1">
+        <v>175</v>
+      </c>
+      <c r="C34" s="1">
+        <v>37</v>
+      </c>
+      <c r="D34" s="1">
+        <v>62</v>
+      </c>
+      <c r="E34" s="1">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="1">
+        <v>280</v>
+      </c>
+      <c r="C35" s="1">
+        <v>210</v>
+      </c>
+      <c r="D35" s="1">
+        <v>215</v>
+      </c>
+      <c r="E35" s="1">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" s="1">
+        <v>512</v>
+      </c>
+      <c r="C36" s="1">
+        <v>33</v>
+      </c>
+      <c r="D36" s="1">
+        <v>157</v>
+      </c>
+      <c r="E36" s="1">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" s="1">
+        <v>223</v>
+      </c>
+      <c r="C37" s="1">
+        <v>11</v>
+      </c>
+      <c r="D37" s="1">
+        <v>58</v>
+      </c>
+      <c r="E37" s="1">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" s="1">
+        <v>740</v>
+      </c>
+      <c r="C38" s="1">
+        <v>23</v>
+      </c>
+      <c r="D38" s="1">
+        <v>321</v>
+      </c>
+      <c r="E38" s="1">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39" s="1">
+        <v>6</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0</v>
+      </c>
+      <c r="E39" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B40" s="1">
+        <v>3655</v>
+      </c>
+      <c r="C40" s="1">
+        <v>479</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1883</v>
+      </c>
+      <c r="E40" s="1">
+        <v>6017</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41" s="1">
+        <v>0</v>
+      </c>
+      <c r="C41" s="1">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0</v>
+      </c>
+      <c r="E41" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42" s="1">
+        <v>1811</v>
+      </c>
+      <c r="C42" s="1">
+        <v>215</v>
+      </c>
+      <c r="D42" s="1">
+        <v>961</v>
+      </c>
+      <c r="E42" s="1">
+        <v>2987</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="1">
+        <v>175</v>
+      </c>
+      <c r="C43" s="1">
+        <v>8</v>
+      </c>
+      <c r="D43" s="1">
+        <v>84</v>
+      </c>
+      <c r="E43" s="1">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B44" s="1">
+        <v>262</v>
+      </c>
+      <c r="C44" s="1">
+        <v>147</v>
+      </c>
+      <c r="D44" s="1">
+        <v>224</v>
+      </c>
+      <c r="E44" s="1">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B45" s="1">
+        <v>476</v>
+      </c>
+      <c r="C45" s="1">
+        <v>38</v>
+      </c>
+      <c r="D45" s="1">
+        <v>220</v>
+      </c>
+      <c r="E45" s="1">
+        <v>734</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B46" s="1">
+        <v>388</v>
+      </c>
+      <c r="C46" s="1">
+        <v>34</v>
+      </c>
+      <c r="D46" s="1">
+        <v>155</v>
+      </c>
+      <c r="E46" s="1">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B47" s="1">
+        <v>543</v>
+      </c>
+      <c r="C47" s="1">
+        <v>36</v>
+      </c>
+      <c r="D47" s="1">
+        <v>239</v>
+      </c>
+      <c r="E47" s="1">
+        <v>818</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B48" s="1">
+        <v>20</v>
+      </c>
+      <c r="C48" s="1">
+        <v>0</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0</v>
+      </c>
+      <c r="E48" s="1">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B49" s="1">
+        <v>14</v>
+      </c>
+      <c r="C49" s="1">
+        <v>0</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0</v>
+      </c>
+      <c r="E49" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50" s="1">
+        <v>1</v>
+      </c>
+      <c r="C50" s="1">
+        <v>0</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0</v>
+      </c>
+      <c r="E50" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B51" s="1">
+        <v>2</v>
+      </c>
+      <c r="C51" s="1">
+        <v>0</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0</v>
+      </c>
+      <c r="E51" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B52" s="1">
+        <v>1</v>
+      </c>
+      <c r="C52" s="1">
+        <v>0</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B53" s="1">
+        <v>2</v>
+      </c>
+      <c r="C53" s="1">
+        <v>0</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0</v>
+      </c>
+      <c r="E53" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B54" s="1">
+        <v>4546</v>
+      </c>
+      <c r="C54" s="1">
+        <v>0</v>
+      </c>
+      <c r="D54" s="1">
+        <v>1469</v>
+      </c>
+      <c r="E54" s="1">
+        <v>6015</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2216</v>
+      </c>
+      <c r="C55" s="1">
+        <v>0</v>
+      </c>
+      <c r="D55" s="1">
+        <v>610</v>
+      </c>
+      <c r="E55" s="1">
+        <v>2826</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="1">
+        <v>253</v>
+      </c>
+      <c r="C56" s="1">
+        <v>0</v>
+      </c>
+      <c r="D56" s="1">
+        <v>61</v>
+      </c>
+      <c r="E56" s="1">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B57" s="1">
+        <v>362</v>
+      </c>
+      <c r="C57" s="1">
+        <v>0</v>
+      </c>
+      <c r="D57" s="1">
+        <v>407</v>
+      </c>
+      <c r="E57" s="1">
+        <v>769</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B58" s="1">
+        <v>549</v>
+      </c>
+      <c r="C58" s="1">
+        <v>0</v>
+      </c>
+      <c r="D58" s="1">
+        <v>180</v>
+      </c>
+      <c r="E58" s="1">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B59" s="1">
+        <v>396</v>
+      </c>
+      <c r="C59" s="1">
+        <v>0</v>
+      </c>
+      <c r="D59" s="1">
+        <v>31</v>
+      </c>
+      <c r="E59" s="1">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" s="1">
+        <v>769</v>
+      </c>
+      <c r="C60" s="1">
+        <v>0</v>
+      </c>
+      <c r="D60" s="1">
+        <v>180</v>
+      </c>
+      <c r="E60" s="1">
+        <v>949</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B61" s="1">
+        <v>1</v>
+      </c>
+      <c r="C61" s="1">
+        <v>0</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0</v>
+      </c>
+      <c r="E61" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B62" s="1">
+        <v>6005</v>
+      </c>
+      <c r="C62" s="1">
+        <v>0</v>
+      </c>
+      <c r="D62" s="1">
+        <v>0</v>
+      </c>
+      <c r="E62" s="1">
+        <v>6005</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B63" s="1">
+        <v>3001</v>
+      </c>
+      <c r="C63" s="1">
+        <v>0</v>
+      </c>
+      <c r="D63" s="1">
+        <v>0</v>
+      </c>
+      <c r="E63" s="1">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B64" s="1">
+        <v>295</v>
+      </c>
+      <c r="C64" s="1">
+        <v>0</v>
+      </c>
+      <c r="D64" s="1">
+        <v>0</v>
+      </c>
+      <c r="E64" s="1">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B65" s="1">
+        <v>725</v>
+      </c>
+      <c r="C65" s="1">
+        <v>0</v>
+      </c>
+      <c r="D65" s="1">
+        <v>0</v>
+      </c>
+      <c r="E65" s="1">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B66" s="1">
+        <v>720</v>
+      </c>
+      <c r="C66" s="1">
+        <v>0</v>
+      </c>
+      <c r="D66" s="1">
+        <v>0</v>
+      </c>
+      <c r="E66" s="1">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B67" s="1">
+        <v>384</v>
+      </c>
+      <c r="C67" s="1">
+        <v>0</v>
+      </c>
+      <c r="D67" s="1">
+        <v>0</v>
+      </c>
+      <c r="E67" s="1">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B68" s="1">
+        <v>880</v>
+      </c>
+      <c r="C68" s="1">
+        <v>0</v>
+      </c>
+      <c r="D68" s="1">
+        <v>0</v>
+      </c>
+      <c r="E68" s="1">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B69" s="1">
+        <v>277</v>
+      </c>
+      <c r="C69" s="1">
+        <v>0</v>
+      </c>
+      <c r="D69" s="1">
+        <v>39</v>
+      </c>
+      <c r="E69" s="1">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B70" s="1">
+        <v>150</v>
+      </c>
+      <c r="C70" s="1">
+        <v>0</v>
+      </c>
+      <c r="D70" s="1">
+        <v>33</v>
+      </c>
+      <c r="E70" s="1">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B71" s="1">
+        <v>122</v>
+      </c>
+      <c r="C71" s="1">
+        <v>0</v>
+      </c>
+      <c r="D71" s="1">
+        <v>6</v>
+      </c>
+      <c r="E71" s="1">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B72" s="1">
+        <v>3</v>
+      </c>
+      <c r="C72" s="1">
+        <v>0</v>
+      </c>
+      <c r="D72" s="1">
+        <v>0</v>
+      </c>
+      <c r="E72" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B73" s="1">
+        <v>1</v>
+      </c>
+      <c r="C73" s="1">
+        <v>0</v>
+      </c>
+      <c r="D73" s="1">
+        <v>0</v>
+      </c>
+      <c r="E73" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B74" s="1">
+        <v>1</v>
+      </c>
+      <c r="C74" s="1">
+        <v>0</v>
+      </c>
+      <c r="D74" s="1">
+        <v>0</v>
+      </c>
+      <c r="E74" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B75" s="1">
+        <v>3529</v>
+      </c>
+      <c r="C75" s="1">
+        <v>374</v>
+      </c>
+      <c r="D75" s="1">
+        <v>2088</v>
+      </c>
+      <c r="E75" s="1">
+        <v>5991</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B76" s="1">
+        <v>1613</v>
+      </c>
+      <c r="C76" s="1">
+        <v>170</v>
+      </c>
+      <c r="D76" s="1">
+        <v>971</v>
+      </c>
+      <c r="E76" s="1">
+        <v>2754</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B77" s="1">
+        <v>217</v>
+      </c>
+      <c r="C77" s="1">
+        <v>11</v>
+      </c>
+      <c r="D77" s="1">
+        <v>95</v>
+      </c>
+      <c r="E77" s="1">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B78" s="1">
+        <v>274</v>
+      </c>
+      <c r="C78" s="1">
+        <v>117</v>
+      </c>
+      <c r="D78" s="1">
+        <v>310</v>
+      </c>
+      <c r="E78" s="1">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B79" s="1">
+        <v>483</v>
+      </c>
+      <c r="C79" s="1">
+        <v>35</v>
+      </c>
+      <c r="D79" s="1">
+        <v>243</v>
+      </c>
+      <c r="E79" s="1">
+        <v>761</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B80" s="1">
+        <v>318</v>
+      </c>
+      <c r="C80" s="1">
+        <v>8</v>
+      </c>
+      <c r="D80" s="1">
+        <v>130</v>
+      </c>
+      <c r="E80" s="1">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B81" s="1">
+        <v>624</v>
+      </c>
+      <c r="C81" s="1">
+        <v>33</v>
+      </c>
+      <c r="D81" s="1">
+        <v>337</v>
+      </c>
+      <c r="E81" s="1">
+        <v>994</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B82" s="1">
+        <v>0</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0</v>
+      </c>
+      <c r="D82" s="1">
+        <v>2</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83" s="1">
+        <v>5825</v>
+      </c>
+      <c r="C83" s="1">
+        <v>0</v>
+      </c>
+      <c r="D83" s="1">
+        <v>0</v>
+      </c>
+      <c r="E83" s="1">
+        <v>5825</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B84" s="1">
+        <v>2926</v>
+      </c>
+      <c r="C84" s="1">
+        <v>0</v>
+      </c>
+      <c r="D84" s="1">
+        <v>0</v>
+      </c>
+      <c r="E84" s="1">
+        <v>2926</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B85" s="1">
+        <v>295</v>
+      </c>
+      <c r="C85" s="1">
+        <v>0</v>
+      </c>
+      <c r="D85" s="1">
+        <v>0</v>
+      </c>
+      <c r="E85" s="1">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B86" s="1">
+        <v>707</v>
+      </c>
+      <c r="C86" s="1">
+        <v>0</v>
+      </c>
+      <c r="D86" s="1">
+        <v>0</v>
+      </c>
+      <c r="E86" s="1">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B87" s="1">
+        <v>612</v>
+      </c>
+      <c r="C87" s="1">
+        <v>0</v>
+      </c>
+      <c r="D87" s="1">
+        <v>0</v>
+      </c>
+      <c r="E87" s="1">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B88" s="1">
+        <v>405</v>
+      </c>
+      <c r="C88" s="1">
+        <v>0</v>
+      </c>
+      <c r="D88" s="1">
+        <v>0</v>
+      </c>
+      <c r="E88" s="1">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B89" s="1">
+        <v>879</v>
+      </c>
+      <c r="C89" s="1">
+        <v>0</v>
+      </c>
+      <c r="D89" s="1">
+        <v>0</v>
+      </c>
+      <c r="E89" s="1">
+        <v>879</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B90" s="1">
+        <v>1</v>
+      </c>
+      <c r="C90" s="1">
+        <v>0</v>
+      </c>
+      <c r="D90" s="1">
+        <v>0</v>
+      </c>
+      <c r="E90" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" s="1">
+        <v>4933</v>
+      </c>
+      <c r="C91" s="1">
+        <v>0</v>
+      </c>
+      <c r="D91" s="1">
+        <v>1192</v>
+      </c>
+      <c r="E91" s="1">
+        <v>6125</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B92" s="1">
+        <v>2509</v>
+      </c>
+      <c r="C92" s="1">
+        <v>0</v>
+      </c>
+      <c r="D92" s="1">
+        <v>535</v>
+      </c>
+      <c r="E92" s="1">
+        <v>3044</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B93" s="1">
+        <v>232</v>
+      </c>
+      <c r="C93" s="1">
+        <v>0</v>
+      </c>
+      <c r="D93" s="1">
+        <v>61</v>
+      </c>
+      <c r="E93" s="1">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B94" s="1">
+        <v>336</v>
+      </c>
+      <c r="C94" s="1">
+        <v>0</v>
+      </c>
+      <c r="D94" s="1">
+        <v>297</v>
+      </c>
+      <c r="E94" s="1">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="B95" s="1">
+        <v>628</v>
+      </c>
+      <c r="C95" s="1">
+        <v>0</v>
+      </c>
+      <c r="D95" s="1">
+        <v>123</v>
+      </c>
+      <c r="E95" s="1">
+        <v>751</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B96" s="1">
+        <v>291</v>
+      </c>
+      <c r="C96" s="1">
+        <v>0</v>
+      </c>
+      <c r="D96" s="1">
+        <v>29</v>
+      </c>
+      <c r="E96" s="1">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B97" s="1">
+        <v>931</v>
+      </c>
+      <c r="C97" s="1">
+        <v>0</v>
+      </c>
+      <c r="D97" s="1">
+        <v>146</v>
+      </c>
+      <c r="E97" s="1">
+        <v>1077</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B98" s="1">
+        <v>6</v>
+      </c>
+      <c r="C98" s="1">
+        <v>0</v>
+      </c>
+      <c r="D98" s="1">
+        <v>1</v>
+      </c>
+      <c r="E98" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B99" s="1">
+        <v>21596</v>
+      </c>
+      <c r="C99" s="1">
+        <v>1577</v>
+      </c>
+      <c r="D99" s="1">
+        <v>7927</v>
+      </c>
+      <c r="E99" s="1">
         <v>21684</v>
       </c>
     </row>
@@ -3557,7 +6630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -3964,8 +7037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>